<commit_message>
Updates to lesson 7
</commit_message>
<xml_diff>
--- a/_lessons/lessons/07_metadata/ImageSheet-Module7.xlsx
+++ b/_lessons/lessons/07_metadata/ImageSheet-Module7.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>image7.jpeg</t>
   </si>
@@ -56,15 +56,9 @@
     <t>image4.jpeg</t>
   </si>
   <si>
-    <t>image37.png</t>
-  </si>
-  <si>
     <t>image33.jpeg</t>
   </si>
   <si>
-    <t>image32.jpeg</t>
-  </si>
-  <si>
     <t>image3.jpeg</t>
   </si>
   <si>
@@ -107,21 +101,6 @@
     <t xml:space="preserve"> right image27.jpeg</t>
   </si>
   <si>
-    <t>left image34.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> center image35.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> right image36.png</t>
-  </si>
-  <si>
-    <t>Left image40.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Right image41.png</t>
-  </si>
-  <si>
     <t>DLC_describe.png</t>
   </si>
   <si>
@@ -165,6 +144,24 @@
   </si>
   <si>
     <t>Globe.jpg</t>
+  </si>
+  <si>
+    <t>DLC.png</t>
+  </si>
+  <si>
+    <t>binoculars.jpg</t>
+  </si>
+  <si>
+    <t>mapPlanning.jpg</t>
+  </si>
+  <si>
+    <t>SBLTER_metadataFields.png</t>
+  </si>
+  <si>
+    <t>SBLTER_Metadata.png</t>
+  </si>
+  <si>
+    <t>SBLTER_attirbutes.png</t>
   </si>
 </sst>
 </file>
@@ -582,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -602,13 +599,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -616,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -624,7 +621,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -640,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -648,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -667,13 +664,13 @@
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -681,13 +678,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -695,7 +692,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -703,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -711,7 +708,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -719,7 +716,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -727,7 +724,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -735,7 +732,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -743,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -751,7 +748,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -759,7 +756,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -767,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -775,7 +772,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -791,7 +788,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -799,13 +796,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -813,7 +810,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -821,7 +818,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -829,7 +826,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -837,10 +834,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -848,7 +845,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -856,7 +853,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -864,97 +861,103 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -962,17 +965,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -980,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -988,7 +991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Final updates to lesson 7
knock on wood i think it’s done
</commit_message>
<xml_diff>
--- a/_lessons/lessons/07_metadata/ImageSheet-Module7.xlsx
+++ b/_lessons/lessons/07_metadata/ImageSheet-Module7.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>image7.jpeg</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>CC0PublicDomain.png</t>
+  </si>
+  <si>
+    <t>fighting.jpg</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -712,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>